<commit_message>
Updated Dm v Dp core promoter comparison data and added new motifs
</commit_message>
<xml_diff>
--- a/Dp_v_Dmel_Stamp/Dp_de_novo_top25_v_Dm.xlsx
+++ b/Dp_v_Dmel_Stamp/Dp_de_novo_top25_v_Dm.xlsx
@@ -114,9 +114,6 @@
     <t>ohler8 (#12)</t>
   </si>
   <si>
-    <t>caudal</t>
-  </si>
-  <si>
     <t>ohler1 (unknown1; #14)</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>Dm Core Significant match</t>
+  </si>
+  <si>
+    <t>caudal (#3)</t>
   </si>
 </sst>
 </file>
@@ -579,27 +579,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -959,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -981,7 +961,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -990,31 +970,31 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1025,7 +1005,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>1.03</v>
@@ -1034,23 +1014,23 @@
         <v>33.200000000000003</v>
       </c>
       <c r="F2">
-        <f>E2-50</f>
+        <f t="shared" ref="F2:F26" si="0">E2-50</f>
         <v>-16.799999999999997</v>
       </c>
       <c r="G2" s="6">
         <v>9.9999999999999994E-37</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="3">
         <v>7.8074000000000004E-11</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L2" s="8">
         <v>4.1700000000000001E-3</v>
@@ -1064,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>6.52</v>
@@ -1073,11 +1053,11 @@
         <v>23.7</v>
       </c>
       <c r="F3">
-        <f>E3-50</f>
+        <f t="shared" si="0"/>
         <v>-26.3</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -1086,10 +1066,10 @@
         <v>7.4780000000000004E-10</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L3" s="8">
         <v>1.3499999999999999E-5</v>
@@ -1103,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>16.59</v>
@@ -1112,7 +1092,7 @@
         <v>47.5</v>
       </c>
       <c r="F4">
-        <f>E4-50</f>
+        <f t="shared" si="0"/>
         <v>-2.5</v>
       </c>
       <c r="G4" s="6">
@@ -1125,10 +1105,10 @@
         <v>8.3799999999999996E-9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L4" s="8">
         <v>8.9700000000000005E-3</v>
@@ -1142,7 +1122,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>3.42</v>
@@ -1151,7 +1131,7 @@
         <v>24.6</v>
       </c>
       <c r="F5">
-        <f>E5-50</f>
+        <f t="shared" si="0"/>
         <v>-25.4</v>
       </c>
       <c r="G5" s="6">
@@ -1164,10 +1144,10 @@
         <v>5.7615999999999998E-8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L5" s="8">
         <v>6.3400000000000001E-4</v>
@@ -1181,7 +1161,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>1.06</v>
@@ -1190,7 +1170,7 @@
         <v>25.1</v>
       </c>
       <c r="F6">
-        <f>E6-50</f>
+        <f t="shared" si="0"/>
         <v>-24.9</v>
       </c>
       <c r="G6" s="6">
@@ -1203,10 +1183,10 @@
         <v>4.1170000000000001E-7</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L6" s="8">
         <v>7.28E-3</v>
@@ -1220,7 +1200,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>0.99</v>
@@ -1229,7 +1209,7 @@
         <v>24.3</v>
       </c>
       <c r="F7">
-        <f>E7-50</f>
+        <f t="shared" si="0"/>
         <v>-25.7</v>
       </c>
       <c r="G7" s="6">
@@ -1242,10 +1222,10 @@
         <v>3.5228E-6</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L7" s="8">
         <v>2.5999999999999998E-5</v>
@@ -1259,7 +1239,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>0.24</v>
@@ -1268,23 +1248,23 @@
         <v>42.6</v>
       </c>
       <c r="F8">
-        <f>E8-50</f>
+        <f t="shared" si="0"/>
         <v>-7.3999999999999986</v>
       </c>
       <c r="G8" s="6">
         <v>1E-35</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="3">
         <v>2.1732000000000001E-5</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L8" s="8">
         <v>5.31E-4</v>
@@ -1298,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>0.99</v>
@@ -1307,7 +1287,7 @@
         <v>28.6</v>
       </c>
       <c r="F9">
-        <f>E9-50</f>
+        <f t="shared" si="0"/>
         <v>-21.4</v>
       </c>
       <c r="G9" s="6">
@@ -1320,10 +1300,10 @@
         <v>3.1262E-5</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L9" s="8">
         <v>1.14E-3</v>
@@ -1337,7 +1317,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>1.03</v>
@@ -1346,7 +1326,7 @@
         <v>42.9</v>
       </c>
       <c r="F10">
-        <f>E10-50</f>
+        <f t="shared" si="0"/>
         <v>-7.1000000000000014</v>
       </c>
       <c r="G10" s="6">
@@ -1359,10 +1339,10 @@
         <v>2.4533999999999998E-4</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L10" s="8">
         <v>2.5200000000000001E-3</v>
@@ -1376,7 +1356,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>0.57999999999999996</v>
@@ -1385,23 +1365,23 @@
         <v>31</v>
       </c>
       <c r="F11">
-        <f>E11-50</f>
+        <f t="shared" si="0"/>
         <v>-19</v>
       </c>
       <c r="G11" s="6">
         <v>1E-35</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="3">
         <v>1.5104999999999999E-3</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L11" s="8">
         <v>4.7199999999999998E-4</v>
@@ -1415,7 +1395,7 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>0.94</v>
@@ -1424,7 +1404,7 @@
         <v>23.8</v>
       </c>
       <c r="F12">
-        <f>E12-50</f>
+        <f t="shared" si="0"/>
         <v>-26.2</v>
       </c>
       <c r="G12" s="6">
@@ -1437,10 +1417,10 @@
         <v>4.3731000000000004E-3</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L12" s="8">
         <v>1.4E-3</v>
@@ -1454,7 +1434,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>2.06</v>
@@ -1463,7 +1443,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="F13">
-        <f>E13-50</f>
+        <f t="shared" si="0"/>
         <v>-16.799999999999997</v>
       </c>
       <c r="G13" s="6">
@@ -1476,10 +1456,10 @@
         <v>4.4048000000000004E-3</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L13" s="8">
         <v>1.63E-5</v>
@@ -1493,7 +1473,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>3.14</v>
@@ -1502,23 +1482,23 @@
         <v>28</v>
       </c>
       <c r="F14">
-        <f>E14-50</f>
+        <f t="shared" si="0"/>
         <v>-22</v>
       </c>
       <c r="G14" s="6">
         <v>9.9999999999999998E-67</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" s="3">
         <v>5.1253000000000002E-3</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L14" s="8">
         <v>2.41E-7</v>
@@ -1532,7 +1512,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15">
         <v>2.14</v>
@@ -1541,23 +1521,23 @@
         <v>38.200000000000003</v>
       </c>
       <c r="F15">
-        <f>E15-50</f>
+        <f t="shared" si="0"/>
         <v>-11.799999999999997</v>
       </c>
       <c r="G15" s="6">
         <v>1E-46</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="3">
         <v>8.4393000000000003E-3</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L15" s="8">
         <v>5.0000000000000001E-4</v>
@@ -1571,7 +1551,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>1.0900000000000001</v>
@@ -1580,7 +1560,7 @@
         <v>27.8</v>
       </c>
       <c r="F16">
-        <f>E16-50</f>
+        <f t="shared" si="0"/>
         <v>-22.2</v>
       </c>
       <c r="G16" s="6">
@@ -1593,10 +1573,10 @@
         <v>1.6098999999999999E-2</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L16" s="8">
         <v>3.3300000000000001E-3</v>
@@ -1610,7 +1590,7 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>0.62</v>
@@ -1619,23 +1599,23 @@
         <v>62.4</v>
       </c>
       <c r="F17">
-        <f>E17-50</f>
+        <f t="shared" si="0"/>
         <v>12.399999999999999</v>
       </c>
       <c r="G17" s="6">
         <v>9.9999999999999993E-105</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="3">
         <v>1.7746000000000001E-2</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L17" s="8">
         <v>5.5099999999999995E-4</v>
@@ -1649,7 +1629,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>2.86</v>
@@ -1658,23 +1638,23 @@
         <v>27.4</v>
       </c>
       <c r="F18">
-        <f>E18-50</f>
+        <f t="shared" si="0"/>
         <v>-22.6</v>
       </c>
       <c r="G18" s="6">
         <v>9.9999999999999998E-121</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="I18" s="3">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L18" s="8">
         <v>9.2099999999999994E-3</v>
@@ -1688,7 +1668,7 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>0.15</v>
@@ -1697,23 +1677,23 @@
         <v>45.3</v>
       </c>
       <c r="F19">
-        <f>E19-50</f>
+        <f t="shared" si="0"/>
         <v>-4.7000000000000028</v>
       </c>
       <c r="G19" s="6">
         <v>9.9999999999999993E-35</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="3">
         <v>3.1029999999999999E-2</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L19" s="8">
         <v>5.6600000000000001E-3</v>
@@ -1727,7 +1707,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>1.25</v>
@@ -1736,23 +1716,23 @@
         <v>45.5</v>
       </c>
       <c r="F20">
-        <f>E20-50</f>
+        <f t="shared" si="0"/>
         <v>-4.5</v>
       </c>
       <c r="G20" s="6">
         <v>9.9999999999999994E-68</v>
       </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" s="3">
         <v>3.1528E-2</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L20" s="8">
         <v>7.9000000000000008E-3</v>
@@ -1766,7 +1746,7 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>1.55</v>
@@ -1775,23 +1755,23 @@
         <v>32</v>
       </c>
       <c r="F21">
-        <f>E21-50</f>
+        <f t="shared" si="0"/>
         <v>-18</v>
       </c>
       <c r="G21" s="6">
         <v>1E-62</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="3">
         <v>3.3936000000000001E-2</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L21" s="8">
         <v>3.6999999999999998E-5</v>
@@ -1805,7 +1785,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22">
         <v>2.98</v>
@@ -1814,23 +1794,23 @@
         <v>35.799999999999997</v>
       </c>
       <c r="F22">
-        <f>E22-50</f>
+        <f t="shared" si="0"/>
         <v>-14.200000000000003</v>
       </c>
       <c r="G22" s="6">
         <v>1E-73</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I22" s="3">
         <v>3.4477000000000001E-2</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L22" s="8">
         <v>3.0800000000000002E-6</v>
@@ -1844,7 +1824,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <v>0.33</v>
@@ -1853,7 +1833,7 @@
         <v>23.9</v>
       </c>
       <c r="F23">
-        <f>E23-50</f>
+        <f t="shared" si="0"/>
         <v>-26.1</v>
       </c>
       <c r="G23" s="6">
@@ -1866,10 +1846,10 @@
         <v>5.8401000000000002E-2</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L23" s="8">
         <v>4.6400000000000003E-5</v>
@@ -1883,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24">
         <v>10.33</v>
@@ -1892,11 +1872,11 @@
         <v>39.700000000000003</v>
       </c>
       <c r="F24">
-        <f>E24-50</f>
+        <f t="shared" si="0"/>
         <v>-10.299999999999997</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H24" t="s">
         <v>27</v>
@@ -1905,10 +1885,10 @@
         <v>6.2300000000000001E-2</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L24" s="8">
         <v>5.4199999999999995E-4</v>
@@ -1922,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="4">
         <v>8.99</v>
@@ -1931,23 +1911,23 @@
         <v>36.5</v>
       </c>
       <c r="F25">
-        <f>E25-50</f>
+        <f t="shared" si="0"/>
         <v>-13.5</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" s="3">
         <v>0.13580999999999999</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L25" s="8">
         <v>1.9599999999999999E-3</v>
@@ -1961,7 +1941,7 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26">
         <v>1.22</v>
@@ -1970,23 +1950,23 @@
         <v>24.7</v>
       </c>
       <c r="F26">
-        <f>E26-50</f>
+        <f t="shared" si="0"/>
         <v>-25.3</v>
       </c>
       <c r="G26" s="6">
         <v>9.9999999999999997E-73</v>
       </c>
       <c r="H26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I26" s="3">
         <v>0.19761000000000001</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L26" s="8">
         <v>1.5900000000000001E-3</v>
@@ -1998,13 +1978,13 @@
     <sortCondition ref="L2:L26"/>
   </sortState>
   <conditionalFormatting sqref="I2:I26">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>